<commit_message>
#89 fix MISS02P001 [templete]
</commit_message>
<xml_diff>
--- a/WEBAPP/Uploads/Template/MIS/MISS02TP001.xlsx
+++ b/WEBAPP/Uploads/Template/MIS/MISS02TP001.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\po.klinmala\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F882D79-7AC8-4AA4-A4CC-0E6C7A4EFA1A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B56801D-A635-4123-8CA8-97A6D8D01489}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{B9E47974-AEB2-4CAE-8C4E-27014A2828A3}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" activeTab="1" xr2:uid="{B9E47974-AEB2-4CAE-8C4E-27014A2828A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Descrition" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
   <si>
     <t>Year</t>
   </si>
@@ -33,9 +34,6 @@
     <t>Deployment date</t>
   </si>
   <si>
-    <t>Type day</t>
-  </si>
-  <si>
     <t>D</t>
   </si>
   <si>
@@ -58,6 +56,66 @@
   </si>
   <si>
     <t>30/05/2019</t>
+  </si>
+  <si>
+    <t>Deploy Program</t>
+  </si>
+  <si>
+    <t>Deplot For User</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>Type Day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H    </t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>วันหยุด</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saturday Working </t>
+  </si>
+  <si>
+    <t>วันทำงานที่ได้รับมอบหมาย</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S    </t>
+  </si>
+  <si>
+    <t>Send Program Package</t>
+  </si>
+  <si>
+    <t>วันส่งไฟล์แพคเกจ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I    </t>
+  </si>
+  <si>
+    <t>Deployment on PROD/QA.</t>
+  </si>
+  <si>
+    <t>วันส่งมอบบนเครื่อง PROD/QA.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D    </t>
+  </si>
+  <si>
+    <t>V-Smart infrom issue no deployment</t>
+  </si>
+  <si>
+    <t>วันที่วีสมาร์ทส่งมอบ</t>
   </si>
 </sst>
 </file>
@@ -483,18 +541,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCD81DC-E102-4BB0-92AD-D5C5E272544F}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:5">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -502,66 +561,148 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="D5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71D7669-F80E-44EE-84BF-5EB3625F59DA}">
+  <dimension ref="B6:E10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetData>
+    <row r="6" spans="2:5">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5">
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5">
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5">
+      <c r="B9" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="2:5">
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merge #177 - #199
</commit_message>
<xml_diff>
--- a/WEBAPP/Uploads/Template/MIS/MISS02TP001.xlsx
+++ b/WEBAPP/Uploads/Template/MIS/MISS02TP001.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\po.klinmala\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B56801D-A635-4123-8CA8-97A6D8D01489}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03565C15-B07A-4376-AB41-293C53C81956}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" activeTab="1" xr2:uid="{B9E47974-AEB2-4CAE-8C4E-27014A2828A3}"/>
+    <workbookView xWindow="5304" yWindow="1728" windowWidth="17292" windowHeight="8964" xr2:uid="{B9E47974-AEB2-4CAE-8C4E-27014A2828A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
   <si>
     <t>Year</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Deployment date</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
@@ -116,6 +113,12 @@
   </si>
   <si>
     <t>วันที่วีสมาร์ทส่งมอบ</t>
+  </si>
+  <si>
+    <t>App Code</t>
+  </si>
+  <si>
+    <t>T001</t>
   </si>
 </sst>
 </file>
@@ -541,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CCD81DC-E102-4BB0-92AD-D5C5E272544F}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -553,82 +556,100 @@
     <col min="3" max="5" width="13.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>14</v>
-      </c>
       <c r="D1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="4" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:6">
+      <c r="A3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="1" t="s">
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -641,7 +662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E71D7669-F80E-44EE-84BF-5EB3625F59DA}">
   <dimension ref="B6:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
@@ -649,57 +670,57 @@
   <sheetData>
     <row r="6" spans="2:5">
       <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>16</v>
-      </c>
-      <c r="E6" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="7" spans="2:5">
       <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
         <v>21</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>22</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:5">
       <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>25</v>
-      </c>
-      <c r="E9" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:5">
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
         <v>27</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>